<commit_message>
Added script for Edit Topic's Subject and messahe, delete topic and defaultSEtting for General and Security settings
</commit_message>
<xml_diff>
--- a/WebsiteToolbox/testData.xlsx
+++ b/WebsiteToolbox/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="12585" windowHeight="6270" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="12585" windowHeight="6270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="689">
   <si>
     <t>Username</t>
   </si>
@@ -2286,6 +2286,24 @@
   </si>
   <si>
     <t>Insert text for emotion in subject field and verify emotions on floating header on post page after adding new topic</t>
+  </si>
+  <si>
+    <t>Edit Topic's Message  and verify modified message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post new topic from category tab through automation script </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Edit message</t>
+  </si>
+  <si>
+    <t>Edit Topic from floating header  and verify modified name of Topic</t>
+  </si>
+  <si>
+    <t>Testing Modified</t>
+  </si>
+  <si>
+    <t>Delete Topic and verify deleted topic in Topic listing page</t>
   </si>
 </sst>
 </file>
@@ -3533,10 +3551,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3848,7 +3866,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>57</v>
       </c>
@@ -3921,6 +3939,69 @@
       </c>
       <c r="H15" s="5" t="s">
         <v>586</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -6907,7 +6988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>

</xml_diff>